<commit_message>
EPBDS-10767 Revert to the previous list and add only requested due backward compatibility
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10072_ALL_multiple/rules/Tests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10072_ALL_multiple/rules/Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-10072_ALL_multiple\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-10072_ALL_multiple\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DE4229-36F2-4AF2-AC7C-15F937C0F5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1782D-78B8-46A4-A519-32974F448EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -332,6 +332,9 @@
     <t>SA</t>
   </si>
   <si>
+    <t>CS</t>
+  </si>
+  <si>
     <t>SG</t>
   </si>
   <si>
@@ -858,9 +861,6 @@
   </si>
   <si>
     <t>YT-HQ-CN-ISK-GRE-APJ-MN-W-01012020-01012020</t>
-  </si>
-  <si>
-    <t>ZW</t>
   </si>
 </sst>
 </file>
@@ -954,7 +954,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1234,30 +1234,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1347,25 +1347,25 @@
         <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
       </c>
       <c r="I17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1376,25 +1376,25 @@
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I18" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>8</v>
       </c>
@@ -1405,25 +1405,25 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1434,25 +1434,25 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G20" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H20" t="s">
         <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -1463,25 +1463,25 @@
         <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H21" t="s">
         <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1492,25 +1492,25 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H22" t="s">
         <v>43</v>
       </c>
       <c r="I22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -1521,25 +1521,25 @@
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1550,25 +1550,25 @@
         <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H24" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -1579,25 +1579,25 @@
         <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H25" t="s">
         <v>56</v>
       </c>
       <c r="I25" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -1608,25 +1608,25 @@
         <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G26" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H26" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I26" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -1637,25 +1637,25 @@
         <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F27" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G27" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I27" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -1666,25 +1666,25 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G28" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H28" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I28" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -1695,25 +1695,25 @@
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H29" t="s">
         <v>64</v>
       </c>
       <c r="I29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1724,25 +1724,25 @@
         <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H30" t="s">
         <v>67</v>
       </c>
       <c r="I30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -1753,25 +1753,25 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G31" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H31" t="s">
         <v>63</v>
       </c>
       <c r="I31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>8</v>
       </c>
@@ -1782,25 +1782,25 @@
         <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G32" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H32" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I32" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -1811,25 +1811,25 @@
         <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G33" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H33" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I33" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1840,25 +1840,25 @@
         <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G34" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H34" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>11</v>
       </c>
@@ -1869,25 +1869,25 @@
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G35" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H35" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>12</v>
       </c>
@@ -1898,25 +1898,25 @@
         <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F36" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G36" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>13</v>
       </c>
@@ -1927,25 +1927,25 @@
         <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G37" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H37" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I37" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>14</v>
       </c>
@@ -1956,25 +1956,25 @@
         <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F38" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G38" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H38" t="s">
         <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>15</v>
       </c>
@@ -1985,25 +1985,25 @@
         <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G39" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H39" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>16</v>
       </c>
@@ -2014,25 +2014,25 @@
         <v>51</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G40" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H40" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I40" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>17</v>
       </c>
@@ -2043,25 +2043,25 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G41" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H41" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I41" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J41" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -2072,25 +2072,25 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G42" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H42" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I42" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -2101,25 +2101,25 @@
         <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F43" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G43" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H43" t="s">
         <v>78</v>
       </c>
       <c r="I43" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>7</v>
       </c>
@@ -2130,25 +2130,25 @@
         <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F44" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G44" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H44" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I44" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -2159,25 +2159,25 @@
         <v>56</v>
       </c>
       <c r="E45" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G45" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H45" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I45" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>9</v>
       </c>
@@ -2188,25 +2188,25 @@
         <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H46" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I46" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>10</v>
       </c>
@@ -2217,25 +2217,25 @@
         <v>58</v>
       </c>
       <c r="E47" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F47" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G47" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H47" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I47" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J47" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>11</v>
       </c>
@@ -2246,25 +2246,25 @@
         <v>59</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F48" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H48" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I48" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>12</v>
       </c>
@@ -2275,25 +2275,25 @@
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F49" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G49" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H49" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J49" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>13</v>
       </c>
@@ -2304,25 +2304,25 @@
         <v>61</v>
       </c>
       <c r="E50" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F50" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G50" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H50" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I50" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J50" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>14</v>
       </c>
@@ -2333,25 +2333,25 @@
         <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F51" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G51" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H51" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I51" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>15</v>
       </c>
@@ -2362,25 +2362,25 @@
         <v>63</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F52" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G52" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H52" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I52" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>16</v>
       </c>
@@ -2391,25 +2391,25 @@
         <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G53" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H53" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I53" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J53" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -2420,25 +2420,25 @@
         <v>65</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F54" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G54" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H54" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J54" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>18</v>
       </c>
@@ -2449,25 +2449,25 @@
         <v>66</v>
       </c>
       <c r="E55" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F55" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G55" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H55" t="s">
         <v>85</v>
       </c>
       <c r="I55" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>6</v>
       </c>
@@ -2478,25 +2478,25 @@
         <v>67</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F56" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H56" t="s">
         <v>90</v>
       </c>
       <c r="I56" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>7</v>
       </c>
@@ -2507,25 +2507,25 @@
         <v>68</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F57" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G57" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I57" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J57" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>8</v>
       </c>
@@ -2536,25 +2536,25 @@
         <v>69</v>
       </c>
       <c r="E58" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F58" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G58" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H58" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I58" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J58" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>9</v>
       </c>
@@ -2565,25 +2565,25 @@
         <v>70</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F59" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G59" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H59" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I59" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J59" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>10</v>
       </c>
@@ -2594,25 +2594,25 @@
         <v>71</v>
       </c>
       <c r="E60" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F60" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G60" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H60" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I60" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J60" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>11</v>
       </c>
@@ -2623,25 +2623,25 @@
         <v>72</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F61" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G61" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H61" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I61" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J61" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>12</v>
       </c>
@@ -2652,25 +2652,25 @@
         <v>73</v>
       </c>
       <c r="E62" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F62" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G62" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H62" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I62" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J62" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>13</v>
       </c>
@@ -2681,25 +2681,25 @@
         <v>74</v>
       </c>
       <c r="E63" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F63" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G63" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H63" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I63" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J63" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>14</v>
       </c>
@@ -2710,25 +2710,25 @@
         <v>75</v>
       </c>
       <c r="E64" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F64" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G64" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H64" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I64" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J64" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>15</v>
       </c>
@@ -2739,25 +2739,25 @@
         <v>76</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F65" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G65" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H65" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I65" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J65" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>16</v>
       </c>
@@ -2768,25 +2768,25 @@
         <v>77</v>
       </c>
       <c r="E66" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F66" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G66" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H66" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I66" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J66" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>17</v>
       </c>
@@ -2797,25 +2797,25 @@
         <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F67" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G67" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H67" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I67" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J67" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>18</v>
       </c>
@@ -2826,25 +2826,25 @@
         <v>79</v>
       </c>
       <c r="E68" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F68" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G68" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H68" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I68" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J68" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>6</v>
       </c>
@@ -2855,25 +2855,25 @@
         <v>80</v>
       </c>
       <c r="E69" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F69" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G69" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H69" t="s">
         <v>28</v>
       </c>
       <c r="I69" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J69" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>7</v>
       </c>
@@ -2884,25 +2884,25 @@
         <v>16</v>
       </c>
       <c r="E70" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F70" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G70" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H70" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I70" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J70" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>8</v>
       </c>
@@ -2913,25 +2913,25 @@
         <v>81</v>
       </c>
       <c r="E71" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F71" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G71" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H71" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I71" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J71" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>9</v>
       </c>
@@ -2942,25 +2942,25 @@
         <v>82</v>
       </c>
       <c r="E72" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F72" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G72" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H72" t="s">
         <v>30</v>
       </c>
       <c r="I72" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J72" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>10</v>
       </c>
@@ -2971,25 +2971,25 @@
         <v>83</v>
       </c>
       <c r="E73" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F73" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G73" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H73" t="s">
         <v>40</v>
       </c>
       <c r="I73" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J73" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>11</v>
       </c>
@@ -3000,25 +3000,25 @@
         <v>84</v>
       </c>
       <c r="E74" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G74" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H74" t="s">
         <v>43</v>
       </c>
       <c r="I74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J74" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>12</v>
       </c>
@@ -3029,25 +3029,25 @@
         <v>85</v>
       </c>
       <c r="E75" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F75" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G75" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H75" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I75" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J75" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>13</v>
       </c>
@@ -3058,25 +3058,25 @@
         <v>86</v>
       </c>
       <c r="E76" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F76" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G76" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H76" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I76" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J76" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>14</v>
       </c>
@@ -3087,25 +3087,25 @@
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F77" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G77" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H77" t="s">
         <v>56</v>
       </c>
       <c r="I77" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J77" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>15</v>
       </c>
@@ -3116,25 +3116,25 @@
         <v>87</v>
       </c>
       <c r="E78" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F78" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G78" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H78" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I78" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J78" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>16</v>
       </c>
@@ -3145,25 +3145,25 @@
         <v>88</v>
       </c>
       <c r="E79" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F79" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G79" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H79" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I79" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J79" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>17</v>
       </c>
@@ -3174,25 +3174,25 @@
         <v>89</v>
       </c>
       <c r="E80" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F80" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G80" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H80" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I80" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J80" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>18</v>
       </c>
@@ -3203,25 +3203,25 @@
         <v>90</v>
       </c>
       <c r="E81" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F81" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G81" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H81" t="s">
         <v>64</v>
       </c>
       <c r="I81" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J81" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>6</v>
       </c>
@@ -3232,25 +3232,25 @@
         <v>91</v>
       </c>
       <c r="E82" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F82" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G82" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H82" t="s">
         <v>67</v>
       </c>
       <c r="I82" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J82" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>7</v>
       </c>
@@ -3261,25 +3261,25 @@
         <v>92</v>
       </c>
       <c r="E83" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F83" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G83" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H83" t="s">
         <v>63</v>
       </c>
       <c r="I83" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J83" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>8</v>
       </c>
@@ -3290,25 +3290,25 @@
         <v>93</v>
       </c>
       <c r="E84" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F84" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G84" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H84" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I84" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J84" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>9</v>
       </c>
@@ -3319,25 +3319,25 @@
         <v>94</v>
       </c>
       <c r="E85" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F85" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G85" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H85" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I85" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J85" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>10</v>
       </c>
@@ -3345,28 +3345,28 @@
         <v>27</v>
       </c>
       <c r="D86" t="s">
-        <v>271</v>
+        <v>95</v>
       </c>
       <c r="E86" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F86" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G86" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H86" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I86" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J86" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>11</v>
       </c>
@@ -3374,28 +3374,28 @@
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E87" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F87" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G87" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H87" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I87" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J87" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>12</v>
       </c>
@@ -3406,25 +3406,25 @@
         <v>15</v>
       </c>
       <c r="E88" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F88" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G88" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H88" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I88" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J88" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>13</v>
       </c>
@@ -3432,28 +3432,28 @@
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E89" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F89" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G89" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H89" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I89" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J89" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>14</v>
       </c>
@@ -3461,28 +3461,28 @@
         <v>27</v>
       </c>
       <c r="D90" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E90" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F90" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G90" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H90" t="s">
         <v>80</v>
       </c>
       <c r="I90" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J90" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>15</v>
       </c>
@@ -3490,28 +3490,28 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E91" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F91" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G91" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H91" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I91" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J91" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>16</v>
       </c>
@@ -3519,28 +3519,28 @@
         <v>27</v>
       </c>
       <c r="D92" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E92" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F92" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G92" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H92" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I92" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J92" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>17</v>
       </c>
@@ -3548,28 +3548,28 @@
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F93" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G93" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H93" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I93" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J93" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>18</v>
       </c>
@@ -3577,28 +3577,28 @@
         <v>27</v>
       </c>
       <c r="D94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E94" t="s">
+        <v>123</v>
+      </c>
+      <c r="F94" t="s">
+        <v>217</v>
+      </c>
+      <c r="G94" t="s">
+        <v>226</v>
+      </c>
+      <c r="H94" t="s">
+        <v>245</v>
+      </c>
+      <c r="I94" t="s">
         <v>101</v>
       </c>
-      <c r="E94" t="s">
-        <v>122</v>
-      </c>
-      <c r="F94" t="s">
-        <v>216</v>
-      </c>
-      <c r="G94" t="s">
-        <v>225</v>
-      </c>
-      <c r="H94" t="s">
-        <v>244</v>
-      </c>
-      <c r="I94" t="s">
-        <v>100</v>
-      </c>
       <c r="J94" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>6</v>
       </c>
@@ -3606,28 +3606,28 @@
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E95" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F95" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G95" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H95" t="s">
         <v>78</v>
       </c>
       <c r="I95" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J95" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>7</v>
       </c>
@@ -3635,28 +3635,28 @@
         <v>27</v>
       </c>
       <c r="D96" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E96" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F96" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G96" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H96" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I96" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J96" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>8</v>
       </c>
@@ -3664,28 +3664,28 @@
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E97" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F97" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G97" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H97" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I97" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J97" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>9</v>
       </c>
@@ -3693,28 +3693,28 @@
         <v>27</v>
       </c>
       <c r="D98" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E98" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F98" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G98" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H98" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I98" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J98" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>10</v>
       </c>
@@ -3722,28 +3722,28 @@
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E99" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F99" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G99" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H99" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I99" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J99" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>11</v>
       </c>
@@ -3751,28 +3751,28 @@
         <v>27</v>
       </c>
       <c r="D100" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E100" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F100" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G100" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H100" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I100" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J100" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>12</v>
       </c>
@@ -3780,28 +3780,28 @@
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E101" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F101" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G101" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H101" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I101" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J101" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>13</v>
       </c>
@@ -3809,28 +3809,28 @@
         <v>27</v>
       </c>
       <c r="D102" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E102" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F102" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G102" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H102" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I102" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J102" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>14</v>
       </c>
@@ -3838,28 +3838,28 @@
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E103" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F103" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G103" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H103" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I103" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J103" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>15</v>
       </c>
@@ -3867,28 +3867,28 @@
         <v>27</v>
       </c>
       <c r="D104" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E104" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F104" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G104" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H104" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I104" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J104" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>16</v>
       </c>
@@ -3896,28 +3896,28 @@
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E105" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F105" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G105" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I105" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J105" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>17</v>
       </c>
@@ -3925,28 +3925,28 @@
         <v>27</v>
       </c>
       <c r="D106" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E106" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F106" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G106" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H106" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I106" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J106" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>18</v>
       </c>
@@ -3954,28 +3954,28 @@
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E107" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F107" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G107" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H107" t="s">
         <v>85</v>
       </c>
       <c r="I107" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J107" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>8</v>
       </c>
@@ -3986,25 +3986,25 @@
         <v>44</v>
       </c>
       <c r="E108" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F108" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G108" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H108" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I108" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J108" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>17</v>
       </c>
@@ -4015,22 +4015,22 @@
         <v>42</v>
       </c>
       <c r="E109" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F109" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G109" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H109" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I109" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J109" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>